<commit_message>
Made changes based upon venue responses. Added analytics
</commit_message>
<xml_diff>
--- a/wineries.xlsx
+++ b/wineries.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="252">
   <si>
     <t>mn-title</t>
   </si>
@@ -3789,10 +3789,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3801,7 +3801,7 @@
     <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3855,8 +3855,11 @@
       <c r="C5" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3867,7 +3870,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -3878,7 +3881,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3889,7 +3892,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -3900,7 +3903,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3922,167 +3925,248 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
       <c r="B15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="19" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
       <c r="B18" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>188</v>
+      </c>
+      <c r="D23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>222</v>
       </c>
       <c r="B24" s="19" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="19"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
       <c r="B29" s="17" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>154</v>
       </c>
       <c r="B30" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>188</v>
+      </c>
+      <c r="D30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
       <c r="B31" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>237</v>
+      </c>
+      <c r="C32" t="s">
+        <v>188</v>
+      </c>
+      <c r="D32" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pull winery location details into sepeate file
</commit_message>
<xml_diff>
--- a/wineries.xlsx
+++ b/wineries.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Dropbox\CLD\Orange House\palisade_wine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clorange\Dropbox\CLD\Orange House\palisade_wine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC2F459-DF62-461A-B0EA-5EEA5623A6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Recovered_Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="255">
   <si>
     <t>mn-title</t>
   </si>
@@ -842,11 +841,20 @@
   <si>
     <t>info@whitewaterhill.com</t>
   </si>
+  <si>
+    <t>Need to upate</t>
+  </si>
+  <si>
+    <t>Verify that I have updated</t>
+  </si>
+  <si>
+    <t>Waiting for respose</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1340,28 +1348,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="38.58203125" customWidth="1"/>
+    <col min="3" max="3" width="38.625" customWidth="1"/>
     <col min="4" max="12" width="9" customWidth="1"/>
     <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.375" style="1" customWidth="1"/>
     <col min="16" max="17" width="9" customWidth="1"/>
-    <col min="18" max="18" width="88.83203125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="88.875" style="14" customWidth="1"/>
     <col min="19" max="20" width="9" hidden="1" customWidth="1"/>
     <col min="21" max="139" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>189</v>
       </c>
@@ -1390,7 +1398,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
         <f>_xlfn.CONCAT("A",C2,"B",E2,"C","D")</f>
         <v>AAlfred Eames CellarsBPaoniaCD</v>
@@ -1449,7 +1457,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>80</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>85</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -1626,7 +1634,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>68</v>
       </c>
@@ -1685,7 +1693,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>36</v>
       </c>
@@ -1744,7 +1752,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>86</v>
       </c>
@@ -1803,7 +1811,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -1862,7 +1870,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1929,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>161</v>
       </c>
@@ -1980,7 +1988,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>15</v>
       </c>
@@ -2039,7 +2047,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>23</v>
       </c>
@@ -2098,7 +2106,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>54</v>
       </c>
@@ -2160,7 +2168,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>77</v>
       </c>
@@ -2222,7 +2230,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>47</v>
       </c>
@@ -2281,7 +2289,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},</v>
       </c>
     </row>
-    <row r="17" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>52</v>
       </c>
@@ -2340,7 +2348,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},</v>
       </c>
     </row>
-    <row r="18" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -2399,7 +2407,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},</v>
       </c>
     </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>87</v>
       </c>
@@ -2458,7 +2466,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},</v>
       </c>
     </row>
-    <row r="20" spans="3:21" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>33</v>
       </c>
@@ -2517,7 +2525,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},</v>
       </c>
     </row>
-    <row r="21" spans="3:21" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:21" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>82</v>
       </c>
@@ -2576,7 +2584,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},</v>
       </c>
     </row>
-    <row r="22" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>42</v>
       </c>
@@ -2635,7 +2643,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},</v>
       </c>
     </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>83</v>
       </c>
@@ -2694,7 +2702,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},</v>
       </c>
     </row>
-    <row r="24" spans="3:21" ht="28.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:21" ht="30" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>79</v>
       </c>
@@ -2753,7 +2761,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},</v>
       </c>
     </row>
-    <row r="25" spans="3:21" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>50</v>
       </c>
@@ -2812,7 +2820,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},</v>
       </c>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>88</v>
       </c>
@@ -2871,7 +2879,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},</v>
       </c>
     </row>
-    <row r="27" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>61</v>
       </c>
@@ -2930,7 +2938,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},</v>
       </c>
     </row>
-    <row r="28" spans="3:21" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>39</v>
       </c>
@@ -2989,7 +2997,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},{"name":"Talon Wines","lat": "39.116621","lng":"-108.36067"},</v>
       </c>
     </row>
-    <row r="29" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>81</v>
       </c>
@@ -3048,7 +3056,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},{"name":"Talon Wines","lat": "39.116621","lng":"-108.36067"},{"name":"The Peachfork","lat": "39.04591","lng":"-108.44237"},</v>
       </c>
     </row>
-    <row r="30" spans="3:21" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:21" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>64</v>
       </c>
@@ -3107,7 +3115,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},{"name":"Talon Wines","lat": "39.116621","lng":"-108.36067"},{"name":"The Peachfork","lat": "39.04591","lng":"-108.44237"},{"name":"Two Rivers Winery","lat": "39.090821","lng":"-108.662153"},</v>
       </c>
     </row>
-    <row r="31" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>154</v>
       </c>
@@ -3166,7 +3174,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},{"name":"Talon Wines","lat": "39.116621","lng":"-108.36067"},{"name":"The Peachfork","lat": "39.04591","lng":"-108.44237"},{"name":"Two Rivers Winery","lat": "39.090821","lng":"-108.662153"},{"name":"Varaison Vineyards and Winery, LLC","lat": "39.111978","lng":"-108.355815"},</v>
       </c>
     </row>
-    <row r="32" spans="3:21" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>18</v>
       </c>
@@ -3225,7 +3233,7 @@
         <v>{"name":"Alfred Eames Cellars","lat": "38.82634","lng":"-107.60381"},{"name":"Avant Vineyards","lat": "39.07861","lng":"-108.41027"},{"name":"Black Bridge Winery","lat": "38.88589","lng":"-107.58253"},{"name":"Carlson Vineyards","lat": "39.07221","lng":"-108.40469"},{"name":"Colorado Cellars Winery","lat": "39.07505","lng":"-108.39373"},{"name":"Colterris Winery","lat": "39.108054","lng":"-108.355876"},{"name":"Cottonwood Cellars","lat": "38.60797","lng":"-108.03621"},{"name":"DeBeque Canyon Winery","lat": "39.105627","lng":"-108.355456"},{"name":"Desert Sun Vineyards","lat": "39.04227","lng":"-108.45359"},{"name":"Garfield Estates Vineyard and Winery","lat": "39.107404","lng":"-108.389369"},{"name":"Grande River Vineyards","lat": "39.117231","lng":"-108.362088"},{"name":"Graystone Winery","lat": "39.091901","lng":"-108.430842"},{"name":"Gubbini Winery","lat": "39.09035","lng":"-108.3667"},{"name":"Hermosa Vineyards","lat": "39.045728","lng":"-108.447431"},{"name":"Maison La Belle Vie Winery","lat": "39.104194","lng":"-108.389553"},{"name":"Meadery of the Rockies","lat": "39.105832","lng":"-108.365821"},{"name":"Mesa Park Vineyards","lat": "39.046375","lng":"-108.436188"},{"name":"Mountain View Winery","lat": "38.60738","lng":"-108.00163"},{"name":"Plum Creek Winery","lat": "39.106845","lng":"-108.365892"},{"name":"Ptarmigan Vineyards","lat": "39.03675","lng":"-108.4749"},{"name":"Red Fox Cellars","lat": "39.10468","lng":"-108.38576"},{"name":"Restoration Vineyards","lat": "39.0846623","lng":"-108.3857671"},{"name":"Shiras Winery","lat": "39.06603","lng":"-108.56488"},{"name":"St Kathryn Cellars","lat": "39.116621","lng":"-108.36067"},{"name":"Stone Cottage Cellars","lat": "38.899693","lng":"-107.577303"},{"name":"Talbott's Mountain Gold LLLP","lat": "39.097046","lng":"-108.349879"},{"name":"Talon Wines","lat": "39.116621","lng":"-108.36067"},{"name":"The Peachfork","lat": "39.04591","lng":"-108.44237"},{"name":"Two Rivers Winery","lat": "39.090821","lng":"-108.662153"},{"name":"Varaison Vineyards and Winery, LLC","lat": "39.111978","lng":"-108.355815"},{"name":"Whitewater Hill Vineyards","lat": "39.03685","lng":"-108.45828"},</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -3288,7 +3296,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:N33">
+  <sortState ref="C2:N33">
     <sortCondition ref="C2:C33"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3297,20 +3305,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -3330,7 +3338,7 @@
         <v>'By Appointment'</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -3350,7 +3358,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment'</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3370,7 +3378,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6'</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3390,7 +3398,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6','10am-5:45pm'</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -3410,7 +3418,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6','10am-5:45pm','Winter: M-F 9 - 4&lt;br&gt;Sat 11 - 5&lt;br&gt;Summer: M-F 9 - 5&lt;br&gt;Sat/Sun 10 - 5'</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3430,7 +3438,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6','10am-5:45pm','Winter: M-F 9 - 4&lt;br&gt;Sat 11 - 5&lt;br&gt;Summer: M-F 9 - 5&lt;br&gt;Sat/Sun 10 - 5','10am - 5pm'</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -3450,7 +3458,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6','10am-5:45pm','Winter: M-F 9 - 4&lt;br&gt;Sat 11 - 5&lt;br&gt;Summer: M-F 9 - 5&lt;br&gt;Sat/Sun 10 - 5','10am - 5pm','By Appointment'</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3470,7 +3478,7 @@
         <v>'By Appointment','May-Sept&lt;br&gt;Fri: 12-5&lt;br&gt;Sat: 11-5&lt;br&gt;Sun: 12-4&lt;br&gt;Mon-Thur: By Appointment','Memorial Day - Halloween&lt;br&gt;10-6','10am-5:45pm','Winter: M-F 9 - 4&lt;br&gt;Sat 11 - 5&lt;br&gt;Summer: M-F 9 - 5&lt;br&gt;Sat/Sun 10 - 5','10am - 5pm','By Appointment','Late April-October&lt;br&gt;Sun - Thurs &lt;br&gt;11 - 6&lt;br&gt;Fri/Sat 11 -7&lt;br&gt;October to late April&lt;br&gt; Sun - Fri Noon- 5&lt;br&gt;Sat 11 -5'</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -3483,7 +3491,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -3496,7 +3504,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3509,7 +3517,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3522,7 +3530,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -3535,7 +3543,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -3548,7 +3556,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -3561,7 +3569,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3574,7 +3582,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -3587,7 +3595,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -3600,7 +3608,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -3613,7 +3621,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -3626,7 +3634,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -3639,7 +3647,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -3652,7 +3660,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -3665,7 +3673,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>222</v>
       </c>
@@ -3678,7 +3686,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -3691,7 +3699,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3704,7 +3712,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3717,7 +3725,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -3730,7 +3738,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -3743,7 +3751,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -3756,7 +3764,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -3769,7 +3777,7 @@
         <v>''</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -3791,20 +3799,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -3814,15 +3822,18 @@
       <c r="C1" t="s">
         <v>188</v>
       </c>
-      <c r="E1">
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1">
         <v>1</v>
       </c>
-      <c r="F1" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=@",E1,"@&gt;",A1,"&lt;/option&gt;")</f>
-        <v>&lt;option value=@1@&gt;Alfred Eames Cellars&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F1,"@&gt;",A1,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -3832,15 +3843,15 @@
       <c r="C2" t="s">
         <v>188</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F32" si="0">_xlfn.CONCAT("&lt;option value=@",E2,"@&gt;",A2,"&lt;/option&gt;")</f>
-        <v>&lt;option value=@2@&gt;Avant Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F2,"@&gt;",A2,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3850,15 +3861,15 @@
       <c r="C3" t="s">
         <v>188</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@3@&gt;Black Bridge Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F3,"@&gt;",A3,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -3868,19 +3879,19 @@
       <c r="C4" t="s">
         <v>188</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@4@&gt;Carlson Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F4,"@&gt;",A4,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="17" t="s">
         <v>227</v>
       </c>
       <c r="C5" t="s">
@@ -3889,15 +3900,15 @@
       <c r="D5" t="s">
         <v>188</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@5@&gt;Colorado Cellars Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F5,"@&gt;",A5,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3907,15 +3918,21 @@
       <c r="C6" t="s">
         <v>188</v>
       </c>
-      <c r="E6">
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@6@&gt;Colterris Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F6,"@&gt;",A6,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -3925,15 +3942,15 @@
       <c r="C7" t="s">
         <v>188</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>7</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@7@&gt;Cottonwood Cellars&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F7,"@&gt;",A7,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3943,15 +3960,21 @@
       <c r="C8" t="s">
         <v>188</v>
       </c>
-      <c r="E8">
+      <c r="D8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" t="s">
+        <v>253</v>
+      </c>
+      <c r="F8">
         <v>8</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@8@&gt;DeBeque Canyon Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F8,"@&gt;",A8,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -3961,15 +3984,15 @@
       <c r="C9" t="s">
         <v>188</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>9</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@9@&gt;Desert Sun Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F9,"@&gt;",A9,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -3979,15 +4002,15 @@
       <c r="C10" t="s">
         <v>188</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>10</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@10@&gt;Garfield Estates Vineyard and Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F10,"@&gt;",A10,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3997,15 +4020,15 @@
       <c r="C11" t="s">
         <v>188</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>11</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@11@&gt;Grande River Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F11,"@&gt;",A11,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4015,15 +4038,18 @@
       <c r="C12" t="s">
         <v>188</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F12">
         <v>12</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@12@&gt;Graystone Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F12,"@&gt;",A12,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -4036,15 +4062,15 @@
       <c r="D13" t="s">
         <v>188</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>13</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@13@&gt;Gubbini Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F13,"@&gt;",A13,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -4057,15 +4083,15 @@
       <c r="D14" t="s">
         <v>188</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>14</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@14@&gt;Hermosa Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F14,"@&gt;",A14,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -4075,15 +4101,15 @@
       <c r="C15" t="s">
         <v>188</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>15</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@15@&gt;Maison La Belle Vie Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F15,"@&gt;",A15,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>52</v>
       </c>
@@ -4093,15 +4119,15 @@
       <c r="C16" t="s">
         <v>188</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>16</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@16@&gt;Meadery of the Rockies&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F16,"@&gt;",A16,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -4114,15 +4140,15 @@
       <c r="D17" t="s">
         <v>188</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>17</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@17@&gt;Mesa Park Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F17,"@&gt;",A17,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -4132,15 +4158,15 @@
       <c r="C18" t="s">
         <v>188</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>18</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@18@&gt;Mountain View Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F18,"@&gt;",A18,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -4150,15 +4176,15 @@
       <c r="C19" t="s">
         <v>188</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>19</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@19@&gt;Plum Creek Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F19,"@&gt;",A19,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -4168,15 +4194,15 @@
       <c r="C20" t="s">
         <v>188</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>20</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@20@&gt;Ptarmigan Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F20,"@&gt;",A20,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -4186,15 +4212,15 @@
       <c r="C21" t="s">
         <v>188</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>21</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@21@&gt;Red Fox Cellars&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F21,"@&gt;",A21,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -4207,15 +4233,15 @@
       <c r="D22" t="s">
         <v>188</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>22</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@22@&gt;Restoration Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F22,"@&gt;",A22,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -4228,15 +4254,15 @@
       <c r="D23" t="s">
         <v>188</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>23</v>
       </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@23@&gt;Shiras Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F23,"@&gt;",A23,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>222</v>
       </c>
@@ -4246,15 +4272,15 @@
       <c r="C24" t="s">
         <v>188</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>24</v>
       </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@24@&gt;StKathryn Cellars&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F24,"@&gt;",A24,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -4264,27 +4290,27 @@
       <c r="C25" t="s">
         <v>188</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>25</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@25@&gt;Stone Cottage Cellars&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F25,"@&gt;",A25,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>26</v>
       </c>
-      <c r="F26" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@26@&gt;Talbott's Mountain Gold LLLP&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F26,"@&gt;",A26,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>39</v>
       </c>
@@ -4292,15 +4318,15 @@
       <c r="C27" t="s">
         <v>188</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>27</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@27@&gt;Talon Wines&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F27,"@&gt;",A27,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -4310,15 +4336,15 @@
       <c r="C28" t="s">
         <v>188</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>28</v>
       </c>
-      <c r="F28" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@28@&gt;The Peachfork&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F28,"@&gt;",A28,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4328,15 +4354,15 @@
       <c r="C29" t="s">
         <v>188</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>29</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@29@&gt;Two Rivers Winery&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F29,"@&gt;",A29,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>154</v>
       </c>
@@ -4349,15 +4375,15 @@
       <c r="D30" t="s">
         <v>188</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>30</v>
       </c>
-      <c r="F30" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@30@&gt;Varaison Vineyards and Winery, LLC&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F30,"@&gt;",A30,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -4367,15 +4393,15 @@
       <c r="C31" t="s">
         <v>188</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>31</v>
       </c>
-      <c r="F31" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@31@&gt;Whitewater Hill Vineyards&lt;/option&gt;</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F31,"@&gt;",A31,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>78</v>
       </c>
@@ -4388,29 +4414,30 @@
       <c r="D32" t="s">
         <v>188</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>32</v>
       </c>
-      <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;option value=@32@&gt;Wine Country Inn&lt;/option&gt;</v>
+      <c r="G32" t="e">
+        <f ca="1">_xlfn.CONCAT("&lt;option value=@",F32,"@&gt;",A32,"&lt;/option&gt;")</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="mailto:avantvineyards@aol.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="B25" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="B28" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="B29" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="B32" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="mailto:avantvineyards@aol.com"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="B25" r:id="rId5"/>
+    <hyperlink ref="B28" r:id="rId6"/>
+    <hyperlink ref="B29" r:id="rId7"/>
+    <hyperlink ref="B32" r:id="rId8"/>
+    <hyperlink ref="B5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <customProperties>
-    <customPr name="SSC_SHEET_GUID" r:id="rId10"/>
+    <customPr name="SSC_SHEET_GUID" r:id="rId11"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>